<commit_message>
feat: OpEx % drivers + DSO/DPO WC schedule
</commit_message>
<xml_diff>
--- a/SaaSV/SaaSV_model_v1.xlsx
+++ b/SaaSV/SaaSV_model_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\quant-summer-2025\SaaSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A035AD9F-B10C-45D6-99AD-E9ACC8BACA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1396BC1-B761-4E26-AA48-1684401610B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{270BAFE9-F160-4EC3-8ED5-C7005A9C532B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Line Item</t>
   </si>
@@ -150,16 +150,32 @@
   </si>
   <si>
     <t>Blue Cells = Inputs</t>
+  </si>
+  <si>
+    <t>A-col label</t>
+  </si>
+  <si>
+    <t>SG&amp;A % of Revenue</t>
+  </si>
+  <si>
+    <t>R&amp;D % of Revenue</t>
+  </si>
+  <si>
+    <t>DSO (days)</t>
+  </si>
+  <si>
+    <t>DPO(days)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0,"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0,"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0,;\(&quot;$&quot;#,##0,\)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -231,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -248,12 +264,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -268,18 +295,14 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -290,7 +313,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -308,13 +331,24 @@
     <xf numFmtId="9" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -650,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836D110D-3FA4-49F2-A362-8303600FBB86}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,31 +697,31 @@
     <col min="5" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14">
         <v>2024</v>
       </c>
-      <c r="C1" s="16">
+      <c r="C1" s="14">
         <v>2025</v>
       </c>
-      <c r="D1" s="16">
+      <c r="D1" s="14">
         <v>2026</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="14">
         <v>2027</v>
       </c>
-      <c r="F1" s="16">
+      <c r="F1" s="14">
         <v>2028</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="20">
         <v>1000</v>
       </c>
       <c r="C2" s="5">
@@ -706,38 +740,38 @@
         <f t="shared" si="0"/>
         <v>2936.2500000000005</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="26"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="21">
         <v>0.6</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="21">
         <v>0.45</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="21">
         <v>0.35</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="21">
         <v>0.25</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="21">
         <v>0.2</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-    </row>
-    <row r="4" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="22">
         <v>4000</v>
       </c>
       <c r="C4" s="6">
@@ -757,30 +791,210 @@
         <v>4502.0352400000002</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <f>B2*B4</f>
         <v>4000000</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <f>C2*C4</f>
         <v>5974000</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <f t="shared" ref="D5:F5" si="2">D2*D4</f>
         <v>8306847.0000000019</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="16">
         <f t="shared" si="2"/>
         <v>10695065.512500003</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="16">
         <f t="shared" si="2"/>
         <v>13219100.973450003</v>
       </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2024</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2025</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2026</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2027</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2028</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="1">
+        <f>B8-0.01</f>
+        <v>0.24</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ref="D8:F8" si="3">C8-0.01</f>
+        <v>0.22999999999999998</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.20999999999999996</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="26">
+        <v>0.18</v>
+      </c>
+      <c r="C9" s="1">
+        <f>B9-0.01</f>
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" ref="D9:F9" si="4">C9-0.01</f>
+        <v>0.15999999999999998</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="4"/>
+        <v>0.14999999999999997</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="4"/>
+        <v>0.13999999999999996</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="32">
+        <v>45</v>
+      </c>
+      <c r="C11" s="31">
+        <f>B11-1</f>
+        <v>44</v>
+      </c>
+      <c r="D11" s="31">
+        <f t="shared" ref="D11:F11" si="5">C11-1</f>
+        <v>43</v>
+      </c>
+      <c r="E11" s="31">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="F11" s="31">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="26">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -796,7 +1010,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,22 +1021,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12">
         <v>2024</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="12">
         <v>2025</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="12">
         <v>2026</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="12">
         <v>2027</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="12">
         <v>2028</v>
       </c>
       <c r="G1" s="1"/>
@@ -833,169 +1047,169 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="27">
         <f>Drivers!B5</f>
         <v>4000000</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="27">
         <f>Drivers!C5</f>
         <v>5974000</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="27">
         <f>Drivers!D5</f>
         <v>8306847.0000000019</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="27">
         <f>Drivers!E5</f>
         <v>10695065.512500003</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="27">
         <f>Drivers!F5</f>
         <v>13219100.973450003</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="8"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="27">
         <f>-B2*0.2</f>
         <v>-800000</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="27">
         <f t="shared" ref="C3:F3" si="0">-C2*0.2</f>
         <v>-1194800</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="27">
         <f t="shared" si="0"/>
         <v>-1661369.4000000004</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="27">
         <f t="shared" si="0"/>
         <v>-2139013.1025000005</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="27">
         <f t="shared" si="0"/>
         <v>-2643820.1946900007</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="28">
         <f>B2+B3</f>
         <v>3200000</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="28">
         <f t="shared" ref="C4:F4" si="1">C2+C3</f>
         <v>4779200</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="28">
         <f t="shared" si="1"/>
         <v>6645477.6000000015</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="28">
         <f t="shared" si="1"/>
         <v>8556052.410000002</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="28">
         <f t="shared" si="1"/>
         <v>10575280.778760003</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7">
-        <f>-B2*0.15</f>
-        <v>-600000</v>
-      </c>
-      <c r="C5" s="7">
-        <f t="shared" ref="C5:F5" si="2">-C2*0.15</f>
-        <v>-896100</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="2"/>
-        <v>-1246027.0500000003</v>
-      </c>
-      <c r="E5" s="7">
-        <f t="shared" si="2"/>
-        <v>-1604259.8268750005</v>
-      </c>
-      <c r="F5" s="7">
-        <f t="shared" si="2"/>
-        <v>-1982865.1460175004</v>
+      <c r="B5" s="27">
+        <f>-Drivers!B8*IncomeStmt!B$2</f>
+        <v>-1000000</v>
+      </c>
+      <c r="C5" s="27">
+        <f>-Drivers!C8*IncomeStmt!C$2</f>
+        <v>-1433760</v>
+      </c>
+      <c r="D5" s="27">
+        <f>-Drivers!D8*IncomeStmt!D$2</f>
+        <v>-1910574.8100000003</v>
+      </c>
+      <c r="E5" s="27">
+        <f>-Drivers!E8*IncomeStmt!E$2</f>
+        <v>-2352914.4127500006</v>
+      </c>
+      <c r="F5" s="27">
+        <f>-Drivers!F8*IncomeStmt!F$2</f>
+        <v>-2776011.2044245</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7">
-        <f>-B2*0.1</f>
-        <v>-400000</v>
-      </c>
-      <c r="C6" s="7">
-        <f t="shared" ref="C6:F6" si="3">-C2*0.1</f>
-        <v>-597400</v>
-      </c>
-      <c r="D6" s="7">
-        <f t="shared" si="3"/>
-        <v>-830684.70000000019</v>
-      </c>
-      <c r="E6" s="7">
-        <f t="shared" si="3"/>
-        <v>-1069506.5512500003</v>
-      </c>
-      <c r="F6" s="7">
-        <f t="shared" si="3"/>
-        <v>-1321910.0973450004</v>
+      <c r="B6" s="27">
+        <f>-Drivers!B$9*IncomeStmt!B$2</f>
+        <v>-720000</v>
+      </c>
+      <c r="C6" s="27">
+        <f>-Drivers!C$9*IncomeStmt!C$2</f>
+        <v>-1015579.9999999999</v>
+      </c>
+      <c r="D6" s="27">
+        <f>-Drivers!D$9*IncomeStmt!D$2</f>
+        <v>-1329095.52</v>
+      </c>
+      <c r="E6" s="27">
+        <f>-Drivers!E$9*IncomeStmt!E$2</f>
+        <v>-1604259.826875</v>
+      </c>
+      <c r="F6" s="27">
+        <f>-Drivers!F$9*IncomeStmt!F$2</f>
+        <v>-1850674.136283</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="28">
         <f>B4+B5+B6</f>
-        <v>2200000</v>
-      </c>
-      <c r="C7" s="11">
-        <f t="shared" ref="C7:F7" si="4">C4+C5+C6</f>
-        <v>3285700</v>
-      </c>
-      <c r="D7" s="11">
-        <f t="shared" si="4"/>
-        <v>4568765.8500000006</v>
-      </c>
-      <c r="E7" s="11">
-        <f t="shared" si="4"/>
-        <v>5882286.0318750013</v>
-      </c>
-      <c r="F7" s="11">
-        <f t="shared" si="4"/>
-        <v>7270505.5353975017</v>
+        <v>1480000</v>
+      </c>
+      <c r="C7" s="28">
+        <f t="shared" ref="C7:F7" si="2">C4+C5+C6</f>
+        <v>2329860</v>
+      </c>
+      <c r="D7" s="28">
+        <f t="shared" si="2"/>
+        <v>3405807.2700000009</v>
+      </c>
+      <c r="E7" s="28">
+        <f t="shared" si="2"/>
+        <v>4598878.1703750016</v>
+      </c>
+      <c r="F7" s="28">
+        <f t="shared" si="2"/>
+        <v>5948595.4380525025</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1005,19 +1219,19 @@
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="25">
-        <v>0</v>
-      </c>
-      <c r="C8" s="25">
-        <v>0</v>
-      </c>
-      <c r="D8" s="25">
-        <v>0</v>
-      </c>
-      <c r="E8" s="25">
-        <v>0</v>
-      </c>
-      <c r="F8" s="25">
+      <c r="B8" s="29">
+        <v>0</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0</v>
+      </c>
+      <c r="D8" s="29">
+        <v>0</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0</v>
+      </c>
+      <c r="F8" s="29">
         <v>0</v>
       </c>
       <c r="G8" s="1"/>
@@ -1025,28 +1239,28 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="28">
         <f>B7-B8</f>
-        <v>2200000</v>
-      </c>
-      <c r="C9" s="11">
-        <f t="shared" ref="C9:F9" si="5">C7-C8</f>
-        <v>3285700</v>
-      </c>
-      <c r="D9" s="11">
-        <f t="shared" si="5"/>
-        <v>4568765.8500000006</v>
-      </c>
-      <c r="E9" s="11">
-        <f t="shared" si="5"/>
-        <v>5882286.0318750013</v>
-      </c>
-      <c r="F9" s="11">
-        <f t="shared" si="5"/>
-        <v>7270505.5353975017</v>
+        <v>1480000</v>
+      </c>
+      <c r="C9" s="28">
+        <f t="shared" ref="C9:F9" si="3">C7-C8</f>
+        <v>2329860</v>
+      </c>
+      <c r="D9" s="28">
+        <f t="shared" si="3"/>
+        <v>3405807.2700000009</v>
+      </c>
+      <c r="E9" s="28">
+        <f t="shared" si="3"/>
+        <v>4598878.1703750016</v>
+      </c>
+      <c r="F9" s="28">
+        <f t="shared" si="3"/>
+        <v>5948595.4380525025</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1056,53 +1270,53 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="27">
         <f>-MAX(0, B9)*0.25</f>
-        <v>-550000</v>
-      </c>
-      <c r="C10" s="7">
-        <f t="shared" ref="C10:F10" si="6">-MAX(0, C9)*0.25</f>
-        <v>-821425</v>
-      </c>
-      <c r="D10" s="7">
-        <f t="shared" si="6"/>
-        <v>-1142191.4625000001</v>
-      </c>
-      <c r="E10" s="7">
-        <f t="shared" si="6"/>
-        <v>-1470571.5079687503</v>
-      </c>
-      <c r="F10" s="7">
-        <f t="shared" si="6"/>
-        <v>-1817626.3838493754</v>
+        <v>-370000</v>
+      </c>
+      <c r="C10" s="27">
+        <f t="shared" ref="C10:F10" si="4">-MAX(0, C9)*0.25</f>
+        <v>-582465</v>
+      </c>
+      <c r="D10" s="27">
+        <f t="shared" si="4"/>
+        <v>-851451.81750000024</v>
+      </c>
+      <c r="E10" s="27">
+        <f t="shared" si="4"/>
+        <v>-1149719.5425937504</v>
+      </c>
+      <c r="F10" s="27">
+        <f t="shared" si="4"/>
+        <v>-1487148.8595131256</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="30">
         <f>B9+B10</f>
-        <v>1650000</v>
-      </c>
-      <c r="C11" s="13">
-        <f t="shared" ref="C11:F11" si="7">C9+C10</f>
-        <v>2464275</v>
-      </c>
-      <c r="D11" s="13">
-        <f t="shared" si="7"/>
-        <v>3426574.3875000002</v>
-      </c>
-      <c r="E11" s="13">
-        <f t="shared" si="7"/>
-        <v>4411714.5239062514</v>
-      </c>
-      <c r="F11" s="13">
-        <f t="shared" si="7"/>
-        <v>5452879.1515481267</v>
+        <v>1110000</v>
+      </c>
+      <c r="C11" s="30">
+        <f t="shared" ref="C11:F11" si="5">C9+C10</f>
+        <v>1747395</v>
+      </c>
+      <c r="D11" s="30">
+        <f t="shared" si="5"/>
+        <v>2554355.4525000006</v>
+      </c>
+      <c r="E11" s="30">
+        <f t="shared" si="5"/>
+        <v>3449158.6277812514</v>
+      </c>
+      <c r="F11" s="30">
+        <f t="shared" si="5"/>
+        <v>4461446.5785393771</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1122,7 +1336,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:I6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,22 +1347,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12">
         <v>2024</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="12">
         <v>2025</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="12">
         <v>2026</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="12">
         <v>2027</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="12">
         <v>2028</v>
       </c>
     </row>
@@ -1156,178 +1370,178 @@
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="25">
+      <c r="B2" s="23">
         <v>100000</v>
       </c>
       <c r="C2" s="7">
         <f>CashFlow!B14</f>
-        <v>1609386.3013698631</v>
+        <v>1015446.5753424657</v>
       </c>
       <c r="D2" s="7">
         <f>CashFlow!C14</f>
-        <v>3907485.8986301371</v>
+        <v>2542728.3178082192</v>
       </c>
       <c r="E2" s="7">
         <f>CashFlow!D14</f>
-        <v>7163940.6112671234</v>
+        <v>4884291.9361986313</v>
       </c>
       <c r="F2" s="7">
         <f>CashFlow!E14</f>
-        <v>11395860.828365978</v>
-      </c>
-      <c r="H2" s="8" t="s">
+        <v>8120721.3157038549</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="8"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="7">
-        <f>(Drivers!B5/365)*30</f>
-        <v>328767.12328767125</v>
+        <f>IncomeStmt!B$2/365*Drivers!B$11</f>
+        <v>493150.68493150681</v>
       </c>
       <c r="C3" s="7">
-        <f>(Drivers!C5/365)*30</f>
-        <v>491013.69863013696</v>
+        <f>IncomeStmt!C$2/365*Drivers!C$11</f>
+        <v>720153.42465753423</v>
       </c>
       <c r="D3" s="7">
-        <f>(Drivers!D5/365)*30</f>
-        <v>682754.54794520559</v>
+        <f>IncomeStmt!D$2/365*Drivers!D$11</f>
+        <v>978614.85205479467</v>
       </c>
       <c r="E3" s="7">
-        <f>(Drivers!E5/365)*30</f>
-        <v>879046.48047945229</v>
+        <f>IncomeStmt!E$2/365*Drivers!E$11</f>
+        <v>1230665.0726712332</v>
       </c>
       <c r="F3" s="7">
-        <f>(Drivers!F5/365)*30</f>
-        <v>1086501.4498726029</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+        <f>IncomeStmt!F$2/365*Drivers!F$11</f>
+        <v>1484885.3148258908</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="23">
         <v>50000</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="23">
         <v>50000</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="23">
         <v>50000</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="23">
         <v>50000</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="23">
         <v>50000</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <f>B2+B3+B4</f>
-        <v>478767.12328767125</v>
-      </c>
-      <c r="C5" s="11">
+        <v>643150.68493150687</v>
+      </c>
+      <c r="C5" s="10">
         <f t="shared" ref="C5:F5" si="0">C2+C3+C4</f>
-        <v>2150400</v>
-      </c>
-      <c r="D5" s="11">
+        <v>1785600</v>
+      </c>
+      <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>4640240.4465753427</v>
-      </c>
-      <c r="E5" s="11">
+        <v>3571343.169863014</v>
+      </c>
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
-        <v>8092987.0917465761</v>
-      </c>
-      <c r="F5" s="11">
+        <v>6164957.008869864</v>
+      </c>
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
-        <v>12532362.278238581</v>
-      </c>
-      <c r="H5" s="26" t="s">
+        <v>9655606.6305297464</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="7">
-        <f>-(IncomeStmt!B3/365)*20</f>
-        <v>43835.616438356163</v>
+        <f>-(IncomeStmt!B$3/365)*Drivers!B$12</f>
+        <v>65753.42465753424</v>
       </c>
       <c r="C6" s="7">
-        <f>-(IncomeStmt!C3/365)*20</f>
-        <v>65468.493150684939</v>
+        <f>-(IncomeStmt!C$3/365)*Drivers!C$12</f>
+        <v>98202.739726027401</v>
       </c>
       <c r="D6" s="7">
-        <f>-(IncomeStmt!D3/365)*20</f>
-        <v>91033.939726027427</v>
+        <f>-(IncomeStmt!D$3/365)*Drivers!D$12</f>
+        <v>136550.90958904114</v>
       </c>
       <c r="E6" s="7">
-        <f>-(IncomeStmt!E3/365)*20</f>
-        <v>117206.19739726029</v>
+        <f>-(IncomeStmt!E$3/365)*Drivers!E$12</f>
+        <v>175809.29609589043</v>
       </c>
       <c r="F6" s="7">
-        <f>-(IncomeStmt!F3/365)*20</f>
-        <v>144866.85998301374</v>
-      </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+        <f>-(IncomeStmt!F$3/365)*Drivers!F$12</f>
+        <v>217300.28997452062</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="25">
-        <v>0</v>
-      </c>
-      <c r="C7" s="25">
-        <v>0</v>
-      </c>
-      <c r="D7" s="25">
-        <v>0</v>
-      </c>
-      <c r="E7" s="25">
-        <v>0</v>
-      </c>
-      <c r="F7" s="25">
+      <c r="B7" s="23">
+        <v>0</v>
+      </c>
+      <c r="C7" s="23">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0</v>
+      </c>
+      <c r="F7" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <f>B5-B6-B7</f>
-        <v>434931.50684931508</v>
-      </c>
-      <c r="C8" s="11">
+        <v>577397.26027397264</v>
+      </c>
+      <c r="C8" s="10">
         <f t="shared" ref="C8:F8" si="1">C5-C6-C7</f>
-        <v>2084931.506849315</v>
-      </c>
-      <c r="D8" s="11">
+        <v>1687397.2602739725</v>
+      </c>
+      <c r="D8" s="10">
         <f t="shared" si="1"/>
-        <v>4549206.506849315</v>
-      </c>
-      <c r="E8" s="11">
+        <v>3434792.260273973</v>
+      </c>
+      <c r="E8" s="10">
         <f t="shared" si="1"/>
-        <v>7975780.8943493161</v>
-      </c>
-      <c r="F8" s="11">
+        <v>5989147.7127739741</v>
+      </c>
+      <c r="F8" s="10">
         <f t="shared" si="1"/>
-        <v>12387495.418255568</v>
+        <v>9438306.3405552264</v>
       </c>
     </row>
   </sheetData>
@@ -1344,7 +1558,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:I6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,22 +1569,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8">
         <v>2024</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="8">
         <v>2025</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="8">
         <v>2026</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="8">
         <v>2027</v>
       </c>
-      <c r="F1" s="9">
+      <c r="F1" s="8">
         <v>2028</v>
       </c>
     </row>
@@ -1378,177 +1592,177 @@
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="27">
         <f>IncomeStmt!B11</f>
-        <v>1650000</v>
-      </c>
-      <c r="C2" s="7">
+        <v>1110000</v>
+      </c>
+      <c r="C2" s="27">
         <f>IncomeStmt!C11</f>
-        <v>2464275</v>
-      </c>
-      <c r="D2" s="7">
+        <v>1747395</v>
+      </c>
+      <c r="D2" s="27">
         <f>IncomeStmt!D11</f>
-        <v>3426574.3875000002</v>
-      </c>
-      <c r="E2" s="7">
+        <v>2554355.4525000006</v>
+      </c>
+      <c r="E2" s="27">
         <f>IncomeStmt!E11</f>
-        <v>4411714.5239062514</v>
-      </c>
-      <c r="F2" s="7">
+        <v>3449158.6277812514</v>
+      </c>
+      <c r="F2" s="27">
         <f>IncomeStmt!F11</f>
-        <v>5452879.1515481267</v>
-      </c>
-      <c r="H2" s="8" t="s">
+        <v>4461446.5785393771</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="8"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="25">
-        <v>0</v>
-      </c>
-      <c r="C3" s="25">
-        <v>0</v>
-      </c>
-      <c r="D3" s="25">
-        <v>0</v>
-      </c>
-      <c r="E3" s="25">
-        <v>0</v>
-      </c>
-      <c r="F3" s="25">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="B3" s="29">
+        <v>0</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29">
+        <v>0</v>
+      </c>
+      <c r="E3" s="29">
+        <v>0</v>
+      </c>
+      <c r="F3" s="29">
+        <v>0</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="27">
         <f>-1*(BalanceSheet!C3-BalanceSheet!B3)</f>
-        <v>-162246.57534246572</v>
-      </c>
-      <c r="C4" s="7">
+        <v>-227002.73972602742</v>
+      </c>
+      <c r="C4" s="27">
         <f>-1*(BalanceSheet!D3-BalanceSheet!C3)</f>
-        <v>-191740.84931506863</v>
-      </c>
-      <c r="D4" s="7">
+        <v>-258461.42739726044</v>
+      </c>
+      <c r="D4" s="27">
         <f>-1*(BalanceSheet!E3-BalanceSheet!D3)</f>
-        <v>-196291.93253424671</v>
-      </c>
-      <c r="E4" s="7">
+        <v>-252050.22061643854</v>
+      </c>
+      <c r="E4" s="27">
         <f>-1*(BalanceSheet!F3-BalanceSheet!E3)</f>
-        <v>-207454.96939315065</v>
-      </c>
-      <c r="F4" s="7">
+        <v>-254220.24215465761</v>
+      </c>
+      <c r="F4" s="27">
         <f>-1*(BalanceSheet!G3-BalanceSheet!F3)</f>
-        <v>1086501.4498726029</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+        <v>1484885.3148258908</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="27">
         <f>BalanceSheet!C6-BalanceSheet!B6</f>
-        <v>21632.876712328776</v>
-      </c>
-      <c r="C5" s="7">
+        <v>32449.315068493161</v>
+      </c>
+      <c r="C5" s="27">
         <f>BalanceSheet!D6-BalanceSheet!C6</f>
-        <v>25565.446575342488</v>
-      </c>
-      <c r="D5" s="7">
+        <v>38348.16986301374</v>
+      </c>
+      <c r="D5" s="27">
         <f>BalanceSheet!E6-BalanceSheet!D6</f>
-        <v>26172.257671232859</v>
-      </c>
-      <c r="E5" s="7">
+        <v>39258.386506849289</v>
+      </c>
+      <c r="E5" s="27">
         <f>BalanceSheet!F6-BalanceSheet!E6</f>
-        <v>27660.662585753453</v>
-      </c>
-      <c r="F5" s="7">
+        <v>41490.993878630194</v>
+      </c>
+      <c r="F5" s="27">
         <f>BalanceSheet!G6-BalanceSheet!F6</f>
-        <v>-144866.85998301374</v>
-      </c>
-      <c r="H5" s="26" t="s">
+        <v>-217300.28997452062</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="26"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="28">
         <f>SUM(B2:B5)</f>
-        <v>1509386.3013698631</v>
-      </c>
-      <c r="C6" s="11">
+        <v>915446.57534246566</v>
+      </c>
+      <c r="C6" s="28">
         <f t="shared" ref="C6:F6" si="0">SUM(C2:C5)</f>
-        <v>2298099.597260274</v>
-      </c>
-      <c r="D6" s="11">
+        <v>1527281.7424657533</v>
+      </c>
+      <c r="D6" s="28">
         <f t="shared" si="0"/>
-        <v>3256454.7126369863</v>
-      </c>
-      <c r="E6" s="11">
+        <v>2341563.6183904116</v>
+      </c>
+      <c r="E6" s="28">
         <f t="shared" si="0"/>
-        <v>4231920.2170988536</v>
-      </c>
-      <c r="F6" s="11">
+        <v>3236429.3795052236</v>
+      </c>
+      <c r="F6" s="28">
         <f t="shared" si="0"/>
-        <v>6394513.7414377155</v>
-      </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
+        <v>5729031.6033907467</v>
+      </c>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" spans="1:9" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="25">
-        <v>0</v>
-      </c>
-      <c r="C7" s="25">
-        <v>0</v>
-      </c>
-      <c r="D7" s="25">
-        <v>0</v>
-      </c>
-      <c r="E7" s="25">
-        <v>0</v>
-      </c>
-      <c r="F7" s="25">
+      <c r="B7" s="29">
+        <v>0</v>
+      </c>
+      <c r="C7" s="29">
+        <v>0</v>
+      </c>
+      <c r="D7" s="29">
+        <v>0</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="28">
         <f>B7</f>
         <v>0</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="28">
         <f t="shared" ref="C8:F8" si="1">C7</f>
         <v>0</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1557,19 +1771,19 @@
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="25">
-        <v>0</v>
-      </c>
-      <c r="C9" s="25">
-        <v>0</v>
-      </c>
-      <c r="D9" s="25">
-        <v>0</v>
-      </c>
-      <c r="E9" s="25">
-        <v>0</v>
-      </c>
-      <c r="F9" s="25">
+      <c r="B9" s="29">
+        <v>0</v>
+      </c>
+      <c r="C9" s="29">
+        <v>0</v>
+      </c>
+      <c r="D9" s="29">
+        <v>0</v>
+      </c>
+      <c r="E9" s="29">
+        <v>0</v>
+      </c>
+      <c r="F9" s="29">
         <v>0</v>
       </c>
     </row>
@@ -1577,43 +1791,43 @@
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="25">
-        <v>0</v>
-      </c>
-      <c r="C10" s="25">
-        <v>0</v>
-      </c>
-      <c r="D10" s="25">
-        <v>0</v>
-      </c>
-      <c r="E10" s="25">
-        <v>0</v>
-      </c>
-      <c r="F10" s="25">
+      <c r="B10" s="29">
+        <v>0</v>
+      </c>
+      <c r="C10" s="29">
+        <v>0</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0</v>
+      </c>
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="28">
         <f>B9+B10</f>
         <v>0</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="28">
         <f t="shared" ref="C11:F11" si="2">C9+C10</f>
         <v>0</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1622,75 +1836,75 @@
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="27">
         <f>SUM(B6,B8,B11)</f>
-        <v>1509386.3013698631</v>
-      </c>
-      <c r="C12" s="7">
+        <v>915446.57534246566</v>
+      </c>
+      <c r="C12" s="27">
         <f t="shared" ref="C12:F12" si="3">SUM(C6,C8,C11)</f>
-        <v>2298099.597260274</v>
-      </c>
-      <c r="D12" s="7">
+        <v>1527281.7424657533</v>
+      </c>
+      <c r="D12" s="27">
         <f t="shared" si="3"/>
-        <v>3256454.7126369863</v>
-      </c>
-      <c r="E12" s="7">
+        <v>2341563.6183904116</v>
+      </c>
+      <c r="E12" s="27">
         <f t="shared" si="3"/>
-        <v>4231920.2170988536</v>
-      </c>
-      <c r="F12" s="7">
+        <v>3236429.3795052236</v>
+      </c>
+      <c r="F12" s="27">
         <f t="shared" si="3"/>
-        <v>6394513.7414377155</v>
+        <v>5729031.6033907467</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="27">
         <f>BalanceSheet!B2</f>
         <v>100000</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="27">
         <f>BalanceSheet!C2</f>
-        <v>1609386.3013698631</v>
-      </c>
-      <c r="D13" s="7">
+        <v>1015446.5753424657</v>
+      </c>
+      <c r="D13" s="27">
         <f>BalanceSheet!D2</f>
-        <v>3907485.8986301371</v>
-      </c>
-      <c r="E13" s="7">
+        <v>2542728.3178082192</v>
+      </c>
+      <c r="E13" s="27">
         <f>BalanceSheet!E2</f>
-        <v>7163940.6112671234</v>
-      </c>
-      <c r="F13" s="7">
+        <v>4884291.9361986313</v>
+      </c>
+      <c r="F13" s="27">
         <f>BalanceSheet!F2</f>
-        <v>11395860.828365978</v>
+        <v>8120721.3157038549</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="30">
         <f>B13+B12</f>
-        <v>1609386.3013698631</v>
-      </c>
-      <c r="C14" s="13">
+        <v>1015446.5753424657</v>
+      </c>
+      <c r="C14" s="30">
         <f t="shared" ref="C14:F14" si="4">C13+C12</f>
-        <v>3907485.8986301371</v>
-      </c>
-      <c r="D14" s="13">
+        <v>2542728.3178082192</v>
+      </c>
+      <c r="D14" s="30">
         <f t="shared" si="4"/>
-        <v>7163940.6112671234</v>
-      </c>
-      <c r="E14" s="13">
+        <v>4884291.9361986313</v>
+      </c>
+      <c r="E14" s="30">
         <f t="shared" si="4"/>
-        <v>11395860.828365978</v>
-      </c>
-      <c r="F14" s="13">
+        <v>8120721.3157038549</v>
+      </c>
+      <c r="F14" s="30">
         <f t="shared" si="4"/>
-        <v>17790374.569803692</v>
+        <v>13849752.919094602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>